<commit_message>
data and some R
</commit_message>
<xml_diff>
--- a/Business Statistics/data/s3.xlsx
+++ b/Business Statistics/data/s3.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="7000" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="hours" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,9 @@
     <sheet name="restaurant" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="11" r:id="rId8"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -59,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
   <si>
     <t>Pepsi</t>
   </si>
@@ -67,19 +70,10 @@
     <t>Sprite</t>
   </si>
   <si>
-    <t xml:space="preserve">Diet Coke </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite </t>
-  </si>
-  <si>
     <t xml:space="preserve">Dr. Pepper </t>
   </si>
   <si>
     <t xml:space="preserve">Coke Classic </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pepsi </t>
   </si>
   <si>
     <t>Good</t>
@@ -104,6 +98,51 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Diet Coke</t>
+  </si>
+  <si>
+    <t>Count of Diet Coke</t>
+  </si>
+  <si>
+    <t>10-14</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>25-29</t>
+  </si>
+  <si>
+    <t>30-34</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>var</t>
   </si>
 </sst>
 </file>
@@ -165,7 +204,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -195,11 +234,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -214,6 +299,27 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -228,11 +334,429 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>audit!$D$5:$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10-14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15-19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25-29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30-34</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>audit!$E$5:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2104680392"/>
+        <c:axId val="-2099659400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2104680392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2099659400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2099659400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2104680392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Francisco Rosales" refreshedDate="43625.382932986111" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="48">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A2:A50" sheet="softdrinks"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="Diet Coke" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Pepsi"/>
+        <s v="Diet Coke"/>
+        <s v="Coke Classic "/>
+        <s v="Dr. Pepper "/>
+        <s v="Sprite"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="48">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="E4:K6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Diet Coke" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,88 +1083,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <f>AVERAGE(A1:A200)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <f>MEDIAN(A1:A200)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <f>MODE(A1:A200)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>88</v>
       </c>
@@ -1579,97 +2124,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F7" sqref="F7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="6" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2">
+        <v>7</v>
+      </c>
+      <c r="H6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="I6" s="2">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="K6" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f>F6/$K6</f>
+        <v>0.375</v>
+      </c>
+      <c r="G7">
+        <f>G6/$K6</f>
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="H7">
+        <f>H6/$K6</f>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="I7">
+        <f>I6/$K6</f>
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="J7">
+        <f>J6/$K6</f>
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -1679,27 +2299,27 @@
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -1714,17 +2334,17 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -1734,7 +2354,7 @@
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -1744,7 +2364,7 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -1754,7 +2374,7 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:1">
@@ -1764,17 +2384,17 @@
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -1784,17 +2404,17 @@
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:1">
@@ -1819,12 +2439,12 @@
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -1834,7 +2454,7 @@
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1850,90 +2470,120 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>23</v>
       </c>
@@ -1961,6 +2611,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1971,90 +2622,112 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <f>STDEV(A1:A50)</f>
+        <v>18.858051926139652</v>
+      </c>
+      <c r="E2">
+        <f>D2^2</f>
+        <v>355.6261224489794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <f>VAR(A1:A50)</f>
+        <v>355.62612244897946</v>
+      </c>
+      <c r="F3">
+        <f>E2-D3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>82</v>
       </c>
@@ -2326,17 +2999,17 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2442,15 +3115,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>18</v>
@@ -2458,7 +3131,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>22</v>
@@ -2466,7 +3139,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>28</v>
@@ -2474,7 +3147,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>38</v>
@@ -2482,7 +3155,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>33</v>
@@ -2490,7 +3163,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>28</v>
@@ -2498,7 +3171,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -2506,7 +3179,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>11</v>
@@ -2514,7 +3187,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>23</v>
@@ -2522,7 +3195,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>13</v>

</xml_diff>